<commit_message>
cleaned diagram & notified not imported samples
</commit_message>
<xml_diff>
--- a/dist/PerSAIDs.xlsx
+++ b/dist/PerSAIDs.xlsx
@@ -4465,61 +4465,61 @@
     <t>https://www.w3.org/TR/vocab-dcat-3/#Class:Catalog</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42883</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C45677</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C15607</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42883</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C45677</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/SCDO_0002829</t>
   </si>
   <si>
+    <t>http://www.ebi.ac.uk/efo/EFO_0005518</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C16977</t>
   </si>
   <si>
-    <t>http://www.ebi.ac.uk/efo/EFO_0005518</t>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25365</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42614</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25714</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C64917</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/data_3273</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C142495</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164024</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171191</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C49100</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142495</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25365</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C64917</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164024</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42614</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25714</t>
-  </si>
-  <si>
-    <t>http://edamontology.org/data_3273</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171191</t>
   </si>
   <si>
     <t>dcat</t>
@@ -27762,10 +27762,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>1482</v>
@@ -27782,10 +27782,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>1483</v>
@@ -27802,10 +27802,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>1484</v>
@@ -27842,16 +27842,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>1486</v>
       </c>
       <c r="D8" t="s">
-        <v>1502</v>
+        <v>1504</v>
       </c>
       <c r="E8" t="s">
         <v>1506</v>
@@ -27862,16 +27862,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>1487</v>
       </c>
       <c r="D9" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="E9" t="s">
         <v>1506</v>
@@ -27882,10 +27882,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="B10" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>1488</v>
@@ -27902,10 +27902,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>1455</v>
+        <v>1461</v>
       </c>
       <c r="B11" t="s">
-        <v>1455</v>
+        <v>1461</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>1489</v>
@@ -27922,10 +27922,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="B12" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>1490</v>
@@ -27942,10 +27942,10 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>1460</v>
+        <v>1465</v>
       </c>
       <c r="B13" t="s">
-        <v>1460</v>
+        <v>1465</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>1491</v>
@@ -27982,16 +27982,16 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="B15" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>1493</v>
       </c>
       <c r="D15" t="s">
-        <v>1502</v>
+        <v>1505</v>
       </c>
       <c r="E15" t="s">
         <v>1506</v>
@@ -28002,10 +28002,10 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>1461</v>
+        <v>1455</v>
       </c>
       <c r="B16" t="s">
-        <v>1461</v>
+        <v>1455</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>1494</v>
@@ -28022,10 +28022,10 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>1466</v>
+        <v>1456</v>
       </c>
       <c r="B17" t="s">
-        <v>1466</v>
+        <v>1456</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>1495</v>
@@ -28042,16 +28042,16 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>1463</v>
+        <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>1463</v>
+        <v>107</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>1496</v>
+        <v>1486</v>
       </c>
       <c r="D18" t="s">
-        <v>1502</v>
+        <v>1504</v>
       </c>
       <c r="E18" t="s">
         <v>1506</v>
@@ -28062,16 +28062,16 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>1454</v>
+        <v>1466</v>
       </c>
       <c r="B19" t="s">
-        <v>1454</v>
+        <v>1466</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="D19" t="s">
-        <v>1505</v>
+        <v>1502</v>
       </c>
       <c r="E19" t="s">
         <v>1506</v>
@@ -28082,13 +28082,13 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>1465</v>
+        <v>1458</v>
       </c>
       <c r="B20" t="s">
-        <v>1465</v>
+        <v>1458</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="D20" t="s">
         <v>1502</v>
@@ -28102,13 +28102,13 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="B21" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="D21" t="s">
         <v>1502</v>
@@ -28122,16 +28122,16 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>1459</v>
       </c>
       <c r="B22" t="s">
-        <v>107</v>
+        <v>1459</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>1487</v>
+        <v>1499</v>
       </c>
       <c r="D22" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="E22" t="s">
         <v>1506</v>
@@ -28142,10 +28142,10 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>1458</v>
+        <v>1464</v>
       </c>
       <c r="B23" t="s">
-        <v>1458</v>
+        <v>1464</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>1500</v>

</xml_diff>

<commit_message>
changed file in experiment set and add metadata
</commit_message>
<xml_diff>
--- a/dist/PerSAIDs.xlsx
+++ b/dist/PerSAIDs.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3616" uniqueCount="1505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3621" uniqueCount="1505">
   <si>
     <t>psm</t>
   </si>
@@ -91,7 +91,7 @@
     <t>samples</t>
   </si>
   <si>
-    <t>files</t>
+    <t>experimentSets</t>
   </si>
   <si>
     <t>protocols</t>
@@ -247,7 +247,7 @@
     <t>Samples</t>
   </si>
   <si>
-    <t>Files</t>
+    <t>Experiment Sets</t>
   </si>
   <si>
     <t>Sampling Protocols</t>
@@ -388,7 +388,7 @@
     <t>psm_samples</t>
   </si>
   <si>
-    <t>psm_files</t>
+    <t>psm_experimentSets</t>
   </si>
   <si>
     <t>psm_protocols</t>
@@ -2296,9 +2296,6 @@
     <t>belongsToPatient</t>
   </si>
   <si>
-    <t>hasFile</t>
-  </si>
-  <si>
     <t>samplingDate</t>
   </si>
   <si>
@@ -2320,6 +2317,9 @@
     <t>fileURI</t>
   </si>
   <si>
+    <t>metadataURI</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -4225,7 +4225,7 @@
     <t>An individual who is the subject of personal data, persons to whom data refers, and from whom data are collected, processed, and stored.</t>
   </si>
   <si>
-    <t>Files related to sample.</t>
+    <t>Experiment sets related to sample.</t>
   </si>
   <si>
     <t>The date that a sample was collected or obtained.</t>
@@ -4447,67 +4447,67 @@
     <t>https://www.w3.org/TR/vocab-dcat-3/#Class:Catalog</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/SCDO_0002829</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42883</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C45677</t>
+  </si>
+  <si>
     <t>http://www.ebi.ac.uk/efo/EFO_0005518</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42883</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C45677</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/SCDO_0002829</t>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25714</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164024</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C142495</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25365</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/data_3273</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C42614</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C49100</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164024</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C171191</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25365</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25714</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142495</t>
-  </si>
-  <si>
-    <t>http://edamontology.org/data_3273</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C64917</t>
   </si>
   <si>
     <t>dcat</t>
   </si>
   <si>
+    <t>SCDO</t>
+  </si>
+  <si>
+    <t>NCIT</t>
+  </si>
+  <si>
     <t>EFO</t>
-  </si>
-  <si>
-    <t>NCIT</t>
-  </si>
-  <si>
-    <t>SCDO</t>
   </si>
   <si>
     <t>EDAM</t>
@@ -5731,7 +5731,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K716"/>
+  <dimension ref="A1:K717"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -26834,7 +26834,7 @@
         <v>122</v>
       </c>
       <c r="B692" t="s">
-        <v>759</v>
+        <v>24</v>
       </c>
       <c r="C692" t="s">
         <v>783</v>
@@ -26866,7 +26866,7 @@
         <v>122</v>
       </c>
       <c r="B693" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C693" t="s">
         <v>780</v>
@@ -26898,7 +26898,7 @@
         <v>122</v>
       </c>
       <c r="B694" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C694" t="s">
         <v>776</v>
@@ -26930,7 +26930,7 @@
         <v>122</v>
       </c>
       <c r="B695" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C695" t="s">
         <v>776</v>
@@ -26959,7 +26959,7 @@
         <v>123</v>
       </c>
       <c r="B696" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C696" t="s">
         <v>776</v>
@@ -26991,7 +26991,7 @@
         <v>123</v>
       </c>
       <c r="B697" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C697" t="s">
         <v>783</v>
@@ -27026,7 +27026,7 @@
         <v>123</v>
       </c>
       <c r="B698" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C698" t="s">
         <v>782</v>
@@ -27058,7 +27058,7 @@
         <v>123</v>
       </c>
       <c r="B699" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C699" t="s">
         <v>784</v>
@@ -27087,22 +27087,22 @@
     </row>
     <row r="700" spans="1:11">
       <c r="A700" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B700" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C700" t="s">
-        <v>776</v>
+        <v>784</v>
       </c>
       <c r="D700" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="E700" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F700" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G700" t="b">
         <v>0</v>
@@ -27114,7 +27114,7 @@
         <v>1</v>
       </c>
       <c r="K700" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="701" spans="1:11">
@@ -27122,31 +27122,31 @@
         <v>124</v>
       </c>
       <c r="B701" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C701" t="s">
         <v>776</v>
       </c>
       <c r="D701" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="E701" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F701" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G701" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H701" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I701" t="b">
         <v>1</v>
       </c>
       <c r="K701" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="702" spans="1:11">
@@ -27154,13 +27154,13 @@
         <v>124</v>
       </c>
       <c r="B702" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C702" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
       <c r="D702" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="E702" t="b">
         <v>0</v>
@@ -27169,16 +27169,16 @@
         <v>1</v>
       </c>
       <c r="G702" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H702" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I702" t="b">
         <v>1</v>
       </c>
       <c r="K702" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="703" spans="1:11">
@@ -27186,13 +27186,13 @@
         <v>124</v>
       </c>
       <c r="B703" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C703" t="s">
-        <v>776</v>
+        <v>782</v>
       </c>
       <c r="D703" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="E703" t="b">
         <v>0</v>
@@ -27210,7 +27210,7 @@
         <v>1</v>
       </c>
       <c r="K703" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="704" spans="1:11">
@@ -27218,13 +27218,13 @@
         <v>124</v>
       </c>
       <c r="B704" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C704" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="D704" t="s">
-        <v>1408</v>
+        <v>1412</v>
       </c>
       <c r="E704" t="b">
         <v>0</v>
@@ -27242,39 +27242,39 @@
         <v>1</v>
       </c>
       <c r="K704" t="s">
-        <v>1453</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="705" spans="1:11">
       <c r="A705" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B705" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C705" t="s">
-        <v>776</v>
+        <v>784</v>
       </c>
       <c r="D705" t="s">
-        <v>1413</v>
+        <v>1408</v>
       </c>
       <c r="E705" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F705" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G705" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H705" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I705" t="b">
         <v>1</v>
       </c>
       <c r="K705" t="s">
-        <v>1458</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="706" spans="1:11">
@@ -27282,31 +27282,31 @@
         <v>125</v>
       </c>
       <c r="B706" t="s">
-        <v>769</v>
+        <v>772</v>
       </c>
       <c r="C706" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
       <c r="D706" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="E706" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F706" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G706" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H706" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I706" t="b">
         <v>1</v>
       </c>
       <c r="K706" t="s">
-        <v>1456</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="707" spans="1:11">
@@ -27314,13 +27314,13 @@
         <v>125</v>
       </c>
       <c r="B707" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="C707" t="s">
-        <v>776</v>
+        <v>782</v>
       </c>
       <c r="D707" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="E707" t="b">
         <v>0</v>
@@ -27338,7 +27338,7 @@
         <v>1</v>
       </c>
       <c r="K707" t="s">
-        <v>1459</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="708" spans="1:11">
@@ -27346,13 +27346,13 @@
         <v>125</v>
       </c>
       <c r="B708" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C708" t="s">
         <v>776</v>
       </c>
       <c r="D708" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="E708" t="b">
         <v>0</v>
@@ -27370,7 +27370,7 @@
         <v>1</v>
       </c>
       <c r="K708" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="709" spans="1:11">
@@ -27378,13 +27378,13 @@
         <v>125</v>
       </c>
       <c r="B709" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C709" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="D709" t="s">
-        <v>1408</v>
+        <v>1416</v>
       </c>
       <c r="E709" t="b">
         <v>0</v>
@@ -27402,21 +27402,21 @@
         <v>1</v>
       </c>
       <c r="K709" t="s">
-        <v>1453</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="710" spans="1:11">
       <c r="A710" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B710" t="s">
-        <v>772</v>
+        <v>775</v>
       </c>
       <c r="C710" t="s">
-        <v>776</v>
+        <v>784</v>
       </c>
       <c r="D710" t="s">
-        <v>1413</v>
+        <v>1408</v>
       </c>
       <c r="E710" t="b">
         <v>0</v>
@@ -27425,16 +27425,16 @@
         <v>1</v>
       </c>
       <c r="G710" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H710" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I710" t="b">
         <v>1</v>
       </c>
       <c r="K710" t="s">
-        <v>1458</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="711" spans="1:11">
@@ -27442,13 +27442,13 @@
         <v>126</v>
       </c>
       <c r="B711" t="s">
-        <v>769</v>
+        <v>772</v>
       </c>
       <c r="C711" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
       <c r="D711" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="E711" t="b">
         <v>0</v>
@@ -27457,16 +27457,16 @@
         <v>1</v>
       </c>
       <c r="G711" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H711" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I711" t="b">
         <v>1</v>
       </c>
       <c r="K711" t="s">
-        <v>1456</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="712" spans="1:11">
@@ -27474,13 +27474,13 @@
         <v>126</v>
       </c>
       <c r="B712" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="C712" t="s">
-        <v>776</v>
+        <v>782</v>
       </c>
       <c r="D712" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="E712" t="b">
         <v>0</v>
@@ -27498,7 +27498,7 @@
         <v>1</v>
       </c>
       <c r="K712" t="s">
-        <v>1459</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="713" spans="1:11">
@@ -27506,19 +27506,19 @@
         <v>126</v>
       </c>
       <c r="B713" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C713" t="s">
         <v>776</v>
       </c>
       <c r="D713" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="E713" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F713" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G713" t="b">
         <v>0</v>
@@ -27530,7 +27530,7 @@
         <v>1</v>
       </c>
       <c r="K713" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="714" spans="1:11">
@@ -27538,19 +27538,19 @@
         <v>126</v>
       </c>
       <c r="B714" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C714" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="D714" t="s">
-        <v>1408</v>
+        <v>1416</v>
       </c>
       <c r="E714" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F714" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G714" t="b">
         <v>0</v>
@@ -27562,27 +27562,27 @@
         <v>1</v>
       </c>
       <c r="K714" t="s">
-        <v>1453</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="715" spans="1:11">
       <c r="A715" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="B715" t="s">
-        <v>772</v>
+        <v>775</v>
       </c>
       <c r="C715" t="s">
-        <v>776</v>
+        <v>784</v>
       </c>
       <c r="D715" t="s">
-        <v>1413</v>
+        <v>1408</v>
       </c>
       <c r="E715" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F715" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G715" t="b">
         <v>0</v>
@@ -27594,7 +27594,7 @@
         <v>1</v>
       </c>
       <c r="K715" t="s">
-        <v>1458</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="716" spans="1:11">
@@ -27602,30 +27602,62 @@
         <v>105</v>
       </c>
       <c r="B716" t="s">
+        <v>772</v>
+      </c>
+      <c r="C716" t="s">
+        <v>776</v>
+      </c>
+      <c r="D716" t="s">
+        <v>1413</v>
+      </c>
+      <c r="E716" t="b">
+        <v>1</v>
+      </c>
+      <c r="F716" t="b">
+        <v>0</v>
+      </c>
+      <c r="G716" t="b">
+        <v>0</v>
+      </c>
+      <c r="H716" t="b">
+        <v>0</v>
+      </c>
+      <c r="I716" t="b">
+        <v>1</v>
+      </c>
+      <c r="K716" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="717" spans="1:11">
+      <c r="A717" t="s">
+        <v>105</v>
+      </c>
+      <c r="B717" t="s">
         <v>769</v>
       </c>
-      <c r="C716" t="s">
+      <c r="C717" t="s">
         <v>782</v>
       </c>
-      <c r="D716" t="s">
+      <c r="D717" t="s">
         <v>1414</v>
       </c>
-      <c r="E716" t="b">
-        <v>0</v>
-      </c>
-      <c r="F716" t="b">
-        <v>1</v>
-      </c>
-      <c r="G716" t="b">
-        <v>1</v>
-      </c>
-      <c r="H716" t="b">
-        <v>1</v>
-      </c>
-      <c r="I716" t="b">
-        <v>1</v>
-      </c>
-      <c r="K716" t="s">
+      <c r="E717" t="b">
+        <v>0</v>
+      </c>
+      <c r="F717" t="b">
+        <v>1</v>
+      </c>
+      <c r="G717" t="b">
+        <v>1</v>
+      </c>
+      <c r="H717" t="b">
+        <v>1</v>
+      </c>
+      <c r="I717" t="b">
+        <v>1</v>
+      </c>
+      <c r="K717" t="s">
         <v>1456</v>
       </c>
     </row>
@@ -27704,10 +27736,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>1476</v>
@@ -27764,10 +27796,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>1479</v>
@@ -27784,10 +27816,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="B8" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>1480</v>
@@ -27804,10 +27836,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>1455</v>
+        <v>1450</v>
       </c>
       <c r="B9" t="s">
-        <v>1455</v>
+        <v>1450</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>1481</v>
@@ -27844,10 +27876,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="B11" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>1483</v>
@@ -27864,10 +27896,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="B12" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>1484</v>
@@ -27884,16 +27916,16 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>1453</v>
+        <v>103</v>
       </c>
       <c r="B13" t="s">
-        <v>1453</v>
+        <v>103</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>1485</v>
+        <v>1479</v>
       </c>
       <c r="D13" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="E13" t="s">
         <v>1498</v>
@@ -27904,13 +27936,13 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="B14" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="D14" t="s">
         <v>1495</v>
@@ -27924,13 +27956,13 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="B15" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="D15" t="s">
         <v>1495</v>
@@ -27944,16 +27976,16 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>1456</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>1456</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>1476</v>
+        <v>1487</v>
       </c>
       <c r="D16" t="s">
-        <v>1494</v>
+        <v>1495</v>
       </c>
       <c r="E16" t="s">
         <v>1498</v>
@@ -27964,16 +27996,16 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>1457</v>
+        <v>1448</v>
       </c>
       <c r="B17" t="s">
-        <v>1457</v>
+        <v>1448</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>1488</v>
       </c>
       <c r="D17" t="s">
-        <v>1495</v>
+        <v>1497</v>
       </c>
       <c r="E17" t="s">
         <v>1498</v>
@@ -27984,10 +28016,10 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="B18" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>1489</v>
@@ -28004,10 +28036,10 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>1449</v>
+        <v>1458</v>
       </c>
       <c r="B19" t="s">
-        <v>1449</v>
+        <v>1458</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>1490</v>
@@ -28024,16 +28056,16 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>1448</v>
+        <v>1452</v>
       </c>
       <c r="B20" t="s">
-        <v>1448</v>
+        <v>1452</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>1491</v>
       </c>
       <c r="D20" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
       <c r="E20" t="s">
         <v>1498</v>

</xml_diff>

<commit_message>
updated readme & minor changes
</commit_message>
<xml_diff>
--- a/dist/PerSAIDs.xlsx
+++ b/dist/PerSAIDs.xlsx
@@ -4447,64 +4447,64 @@
     <t>https://www.w3.org/TR/vocab-dcat-3/#Class:Catalog</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C45677</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42883</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/SCDO_0002829</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42883</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C45677</t>
-  </si>
-  <si>
     <t>http://www.ebi.ac.uk/efo/EFO_0005518</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C64917</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C142495</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25365</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164024</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C25714</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164024</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/data_3273</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42614</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171191</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C49100</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142495</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25365</t>
-  </si>
-  <si>
-    <t>http://edamontology.org/data_3273</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42614</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C49100</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171191</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C64917</t>
-  </si>
-  <si>
     <t>dcat</t>
   </si>
   <si>
+    <t>NCIT</t>
+  </si>
+  <si>
     <t>SCDO</t>
-  </si>
-  <si>
-    <t>NCIT</t>
   </si>
   <si>
     <t>EFO</t>
@@ -27736,10 +27736,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>1476</v>
@@ -27765,7 +27765,7 @@
         <v>1477</v>
       </c>
       <c r="D5" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="E5" t="s">
         <v>1498</v>
@@ -27776,10 +27776,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>1478</v>
@@ -27816,16 +27816,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>1457</v>
+        <v>1451</v>
       </c>
       <c r="B8" t="s">
-        <v>1457</v>
+        <v>1451</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>1480</v>
       </c>
       <c r="D8" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="E8" t="s">
         <v>1498</v>
@@ -27836,16 +27836,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="B9" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>1481</v>
       </c>
       <c r="D9" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="E9" t="s">
         <v>1498</v>
@@ -27856,16 +27856,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>1460</v>
+        <v>1456</v>
       </c>
       <c r="B10" t="s">
-        <v>1460</v>
+        <v>1456</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>1482</v>
       </c>
       <c r="D10" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="E10" t="s">
         <v>1498</v>
@@ -27876,16 +27876,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>1459</v>
+        <v>1450</v>
       </c>
       <c r="B11" t="s">
-        <v>1459</v>
+        <v>1450</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>1483</v>
       </c>
       <c r="D11" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="E11" t="s">
         <v>1498</v>
@@ -27896,16 +27896,16 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>1449</v>
+        <v>1460</v>
       </c>
       <c r="B12" t="s">
-        <v>1449</v>
+        <v>1460</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>1484</v>
       </c>
       <c r="D12" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="E12" t="s">
         <v>1498</v>
@@ -27916,16 +27916,16 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>1457</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>1457</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>1479</v>
+        <v>1485</v>
       </c>
       <c r="D13" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="E13" t="s">
         <v>1498</v>
@@ -27936,16 +27936,16 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="B14" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>1485</v>
+        <v>1486</v>
       </c>
       <c r="D14" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="E14" t="s">
         <v>1498</v>
@@ -27956,16 +27956,16 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>1454</v>
+        <v>1448</v>
       </c>
       <c r="B15" t="s">
-        <v>1454</v>
+        <v>1448</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>1486</v>
+        <v>1487</v>
       </c>
       <c r="D15" t="s">
-        <v>1495</v>
+        <v>1497</v>
       </c>
       <c r="E15" t="s">
         <v>1498</v>
@@ -27976,16 +27976,16 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="B16" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>1487</v>
+        <v>1488</v>
       </c>
       <c r="D16" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="E16" t="s">
         <v>1498</v>
@@ -27996,16 +27996,16 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>1448</v>
+        <v>1452</v>
       </c>
       <c r="B17" t="s">
-        <v>1448</v>
+        <v>1452</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>1488</v>
+        <v>1489</v>
       </c>
       <c r="D17" t="s">
-        <v>1497</v>
+        <v>1494</v>
       </c>
       <c r="E17" t="s">
         <v>1498</v>
@@ -28016,16 +28016,16 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="B18" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>1489</v>
+        <v>1490</v>
       </c>
       <c r="D18" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="E18" t="s">
         <v>1498</v>
@@ -28042,10 +28042,10 @@
         <v>1458</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>1490</v>
+        <v>1491</v>
       </c>
       <c r="D19" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="E19" t="s">
         <v>1498</v>
@@ -28056,16 +28056,16 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>1452</v>
+        <v>1459</v>
       </c>
       <c r="B20" t="s">
-        <v>1452</v>
+        <v>1459</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>1491</v>
+        <v>1492</v>
       </c>
       <c r="D20" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="E20" t="s">
         <v>1498</v>
@@ -28076,16 +28076,16 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>1451</v>
+        <v>103</v>
       </c>
       <c r="B21" t="s">
-        <v>1451</v>
+        <v>103</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>1492</v>
+        <v>1479</v>
       </c>
       <c r="D21" t="s">
-        <v>1495</v>
+        <v>1496</v>
       </c>
       <c r="E21" t="s">
         <v>1498</v>

</xml_diff>